<commit_message>
addition of testcase screenshots
</commit_message>
<xml_diff>
--- a/Testcases.xlsx
+++ b/Testcases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -206,6 +206,14 @@
   <si>
     <t>Please correct the error below.
 A user with that username already exists.</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>Input:
+Username - admin
+Password - asd</t>
   </si>
 </sst>
 </file>
@@ -290,6 +298,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>500154</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="409576"/>
+          <a:ext cx="3133725" cy="2948078"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>527063</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7343775" y="3629025"/>
+          <a:ext cx="5813438" cy="3457575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>372269</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>67334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="7343775"/>
+          <a:ext cx="5687219" cy="4725059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -555,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,9 +712,10 @@
     <col min="2" max="2" width="29.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="36" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -582,8 +728,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
         <v>16</v>
@@ -591,7 +740,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -605,7 +754,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -619,7 +768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -633,7 +782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -641,13 +790,13 @@
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -661,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
         <v>38</v>
@@ -669,7 +818,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -683,7 +832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -697,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -711,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -725,7 +874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -739,7 +888,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
         <v>39</v>
@@ -747,7 +896,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -761,7 +910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -834,5 +983,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>